<commit_message>
Cambio diagrama de base de datos
</commit_message>
<xml_diff>
--- a/Libro1 las viewer.xlsx
+++ b/Libro1 las viewer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\NetBeansProjects\las_viewer\las-viewer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\NetBeansProjects\desarrollo_las_viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>nombre</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t xml:space="preserve">   15-171-21208</t>
+  </si>
+  <si>
+    <t>Location well</t>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>FLD</t>
   </si>
 </sst>
 </file>
@@ -216,11 +228,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,15 +513,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K17"/>
+  <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
@@ -531,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J2" t="s">
@@ -548,7 +561,7 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1248085</v>
       </c>
       <c r="E3" s="1"/>
@@ -566,7 +579,7 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1910248</v>
       </c>
       <c r="E4" s="1"/>
@@ -635,10 +648,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="5"/>
       <c r="H10" t="s">
         <v>38</v>
       </c>
@@ -730,12 +743,36 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
         <v>45</v>
       </c>
       <c r="I17" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>